<commit_message>
Updated code of print s9, broadcast s9, digital s9 validation
</commit_message>
<xml_diff>
--- a/AP Digital Squarenine/Updated-CSV Validation/CSV Validation -Sept/Data/Config.xlsx
+++ b/AP Digital Squarenine/Updated-CSV Validation/CSV Validation -Sept/Data/Config.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AF5BFB-1F1E-4D72-A070-AFB3DFF21550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D50916-40CD-4E4E-AB96-850FCF202E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="17910" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>